<commit_message>
ID for big pipes added
</commit_message>
<xml_diff>
--- a/data/info/pipes.xlsx
+++ b/data/info/pipes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avner\google drive\Python\Apps\Avner autocad network solver\data\info\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Avner.PALGEY-MAIM\python-avner\Avner autocad network solver\data\info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB374FE5-BD7B-4539-AC16-5F3DAF77391E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C7B1D9ED-A7FF-4D03-98CC-0F364AE1494E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Steel" sheetId="1" r:id="rId1"/>
@@ -23,22 +23,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="20">
   <si>
     <t>ND</t>
   </si>
@@ -104,11 +94,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -130,7 +120,7 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -144,6 +134,18 @@
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="9.6"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="11">
@@ -208,7 +210,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -317,12 +319,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
@@ -390,10 +420,10 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
@@ -402,7 +432,11 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1147,25 +1181,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K136"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+    <sheetView rightToLeft="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="21.375" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
     <col min="4" max="4" width="21" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
-    <col min="6" max="6" width="15.625" customWidth="1"/>
-    <col min="7" max="7" width="13.25" customWidth="1"/>
-    <col min="9" max="9" width="9.625" customWidth="1"/>
-    <col min="10" max="10" width="14.875" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" customWidth="1"/>
+    <col min="9" max="9" width="9.5703125" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -1200,7 +1234,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>13</v>
       </c>
@@ -1233,7 +1267,7 @@
       </c>
       <c r="K2" s="28"/>
     </row>
-    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="17">
         <v>3</v>
       </c>
@@ -1268,7 +1302,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="19">
         <v>3</v>
       </c>
@@ -1301,7 +1335,7 @@
       </c>
       <c r="K4" s="28"/>
     </row>
-    <row r="5" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="19">
         <v>3</v>
       </c>
@@ -1334,7 +1368,7 @@
       </c>
       <c r="K5" s="28"/>
     </row>
-    <row r="6" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="15">
         <v>4</v>
       </c>
@@ -1369,7 +1403,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="15">
         <v>4</v>
       </c>
@@ -1404,7 +1438,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="15">
         <v>4</v>
       </c>
@@ -1437,7 +1471,7 @@
       </c>
       <c r="K8" s="28"/>
     </row>
-    <row r="9" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15">
         <v>4</v>
       </c>
@@ -1470,7 +1504,7 @@
       </c>
       <c r="K9" s="28"/>
     </row>
-    <row r="10" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="19">
         <v>6</v>
       </c>
@@ -1505,7 +1539,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="19">
         <v>6</v>
       </c>
@@ -1540,7 +1574,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="19">
         <v>6</v>
       </c>
@@ -1573,7 +1607,7 @@
       </c>
       <c r="K12" s="28"/>
     </row>
-    <row r="13" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="19">
         <v>6</v>
       </c>
@@ -1606,7 +1640,7 @@
       </c>
       <c r="K13" s="28"/>
     </row>
-    <row r="14" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="19">
         <v>6</v>
       </c>
@@ -1639,7 +1673,7 @@
       </c>
       <c r="K14" s="28"/>
     </row>
-    <row r="15" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="19">
         <v>6</v>
       </c>
@@ -1672,7 +1706,7 @@
       </c>
       <c r="K15" s="28"/>
     </row>
-    <row r="16" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="19">
         <v>6</v>
       </c>
@@ -1705,7 +1739,7 @@
       </c>
       <c r="K16" s="28"/>
     </row>
-    <row r="17" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="15">
         <v>8</v>
       </c>
@@ -1740,7 +1774,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="15">
         <v>8</v>
       </c>
@@ -1775,7 +1809,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="15">
         <v>8</v>
       </c>
@@ -1808,7 +1842,7 @@
       </c>
       <c r="K19" s="28"/>
     </row>
-    <row r="20" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="15">
         <v>8</v>
       </c>
@@ -1841,7 +1875,7 @@
       </c>
       <c r="K20" s="28"/>
     </row>
-    <row r="21" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="15">
         <v>8</v>
       </c>
@@ -1874,7 +1908,7 @@
       </c>
       <c r="K21" s="28"/>
     </row>
-    <row r="22" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="15">
         <v>8</v>
       </c>
@@ -1907,7 +1941,7 @@
       </c>
       <c r="K22" s="28"/>
     </row>
-    <row r="23" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="15">
         <v>8</v>
       </c>
@@ -1940,7 +1974,7 @@
       </c>
       <c r="K23" s="28"/>
     </row>
-    <row r="24" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="15">
         <v>8</v>
       </c>
@@ -1973,7 +2007,7 @@
       </c>
       <c r="K24" s="28"/>
     </row>
-    <row r="25" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="15">
         <v>10</v>
       </c>
@@ -2008,7 +2042,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="15">
         <v>10</v>
       </c>
@@ -2043,7 +2077,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="15">
         <v>10</v>
       </c>
@@ -2076,7 +2110,7 @@
       </c>
       <c r="K27" s="28"/>
     </row>
-    <row r="28" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="15">
         <v>10</v>
       </c>
@@ -2109,7 +2143,7 @@
       </c>
       <c r="K28" s="28"/>
     </row>
-    <row r="29" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="15">
         <v>10</v>
       </c>
@@ -2142,7 +2176,7 @@
       </c>
       <c r="K29" s="28"/>
     </row>
-    <row r="30" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="15">
         <v>10</v>
       </c>
@@ -2175,7 +2209,7 @@
       </c>
       <c r="K30" s="28"/>
     </row>
-    <row r="31" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="15">
         <v>10</v>
       </c>
@@ -2208,7 +2242,7 @@
       </c>
       <c r="K31" s="28"/>
     </row>
-    <row r="32" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="15">
         <v>10</v>
       </c>
@@ -2241,7 +2275,7 @@
       </c>
       <c r="K32" s="28"/>
     </row>
-    <row r="33" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="15">
         <v>10</v>
       </c>
@@ -2274,7 +2308,7 @@
       </c>
       <c r="K33" s="28"/>
     </row>
-    <row r="34" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="15">
         <v>12</v>
       </c>
@@ -2309,7 +2343,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="15">
         <v>12</v>
       </c>
@@ -2344,7 +2378,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="15">
         <v>12</v>
       </c>
@@ -2379,7 +2413,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="15">
         <v>12</v>
       </c>
@@ -2412,7 +2446,7 @@
       </c>
       <c r="K37" s="28"/>
     </row>
-    <row r="38" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="15">
         <v>12</v>
       </c>
@@ -2445,7 +2479,7 @@
       </c>
       <c r="K38" s="28"/>
     </row>
-    <row r="39" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="15">
         <v>12</v>
       </c>
@@ -2478,7 +2512,7 @@
       </c>
       <c r="K39" s="28"/>
     </row>
-    <row r="40" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="15">
         <v>12</v>
       </c>
@@ -2511,7 +2545,7 @@
       </c>
       <c r="K40" s="28"/>
     </row>
-    <row r="41" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="15">
         <v>12</v>
       </c>
@@ -2544,7 +2578,7 @@
       </c>
       <c r="K41" s="28"/>
     </row>
-    <row r="42" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="15">
         <v>12</v>
       </c>
@@ -2577,7 +2611,7 @@
       </c>
       <c r="K42" s="28"/>
     </row>
-    <row r="43" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="15">
         <v>14</v>
       </c>
@@ -2612,7 +2646,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="15">
         <v>14</v>
       </c>
@@ -2647,7 +2681,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="15">
         <v>14</v>
       </c>
@@ -2680,7 +2714,7 @@
       </c>
       <c r="K45" s="28"/>
     </row>
-    <row r="46" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="15">
         <v>14</v>
       </c>
@@ -2713,7 +2747,7 @@
       </c>
       <c r="K46" s="28"/>
     </row>
-    <row r="47" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="15">
         <v>14</v>
       </c>
@@ -2746,7 +2780,7 @@
       </c>
       <c r="K47" s="28"/>
     </row>
-    <row r="48" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="15">
         <v>14</v>
       </c>
@@ -2779,7 +2813,7 @@
       </c>
       <c r="K48" s="28"/>
     </row>
-    <row r="49" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="15">
         <v>14</v>
       </c>
@@ -2812,7 +2846,7 @@
       </c>
       <c r="K49" s="28"/>
     </row>
-    <row r="50" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="15">
         <v>14</v>
       </c>
@@ -2845,7 +2879,7 @@
       </c>
       <c r="K50" s="28"/>
     </row>
-    <row r="51" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="15">
         <v>14</v>
       </c>
@@ -2878,7 +2912,7 @@
       </c>
       <c r="K51" s="28"/>
     </row>
-    <row r="52" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="15">
         <v>16</v>
       </c>
@@ -2913,7 +2947,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="15">
         <v>16</v>
       </c>
@@ -2948,7 +2982,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="15">
         <v>16</v>
       </c>
@@ -2981,7 +3015,7 @@
       </c>
       <c r="K54" s="28"/>
     </row>
-    <row r="55" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="15">
         <v>16</v>
       </c>
@@ -3016,7 +3050,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="15">
         <v>16</v>
       </c>
@@ -3049,7 +3083,7 @@
       </c>
       <c r="K56" s="28"/>
     </row>
-    <row r="57" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="15">
         <v>16</v>
       </c>
@@ -3082,7 +3116,7 @@
       </c>
       <c r="K57" s="28"/>
     </row>
-    <row r="58" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="15">
         <v>16</v>
       </c>
@@ -3115,7 +3149,7 @@
       </c>
       <c r="K58" s="28"/>
     </row>
-    <row r="59" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="15">
         <v>16</v>
       </c>
@@ -3148,7 +3182,7 @@
       </c>
       <c r="K59" s="28"/>
     </row>
-    <row r="60" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="15">
         <v>16</v>
       </c>
@@ -3181,7 +3215,7 @@
       </c>
       <c r="K60" s="28"/>
     </row>
-    <row r="61" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="15">
         <v>18</v>
       </c>
@@ -3216,7 +3250,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="62" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="15">
         <v>18</v>
       </c>
@@ -3251,7 +3285,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="63" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="15">
         <v>18</v>
       </c>
@@ -3284,7 +3318,7 @@
       </c>
       <c r="K63" s="28"/>
     </row>
-    <row r="64" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="15">
         <v>18</v>
       </c>
@@ -3319,7 +3353,7 @@
         <v>1265</v>
       </c>
     </row>
-    <row r="65" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="15">
         <v>18</v>
       </c>
@@ -3352,7 +3386,7 @@
       </c>
       <c r="K65" s="28"/>
     </row>
-    <row r="66" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="15">
         <v>18</v>
       </c>
@@ -3387,7 +3421,7 @@
         <v>1370</v>
       </c>
     </row>
-    <row r="67" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="15">
         <v>18</v>
       </c>
@@ -3420,7 +3454,7 @@
       </c>
       <c r="K67" s="28"/>
     </row>
-    <row r="68" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="15">
         <v>18</v>
       </c>
@@ -3453,7 +3487,7 @@
       </c>
       <c r="K68" s="28"/>
     </row>
-    <row r="69" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="15">
         <v>18</v>
       </c>
@@ -3486,7 +3520,7 @@
       </c>
       <c r="K69" s="28"/>
     </row>
-    <row r="70" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="15">
         <v>20</v>
       </c>
@@ -3521,7 +3555,7 @@
         <v>1140</v>
       </c>
     </row>
-    <row r="71" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="15">
         <v>20</v>
       </c>
@@ -3554,7 +3588,7 @@
       </c>
       <c r="K71" s="28"/>
     </row>
-    <row r="72" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="15">
         <v>20</v>
       </c>
@@ -3587,7 +3621,7 @@
       </c>
       <c r="K72" s="28"/>
     </row>
-    <row r="73" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="15">
         <v>20</v>
       </c>
@@ -3622,7 +3656,7 @@
         <v>1360</v>
       </c>
     </row>
-    <row r="74" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="15">
         <v>20</v>
       </c>
@@ -3655,7 +3689,7 @@
       </c>
       <c r="K74" s="28"/>
     </row>
-    <row r="75" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="15">
         <v>20</v>
       </c>
@@ -3690,7 +3724,7 @@
         <v>1550</v>
       </c>
     </row>
-    <row r="76" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="15">
         <v>20</v>
       </c>
@@ -3723,7 +3757,7 @@
       </c>
       <c r="K76" s="28"/>
     </row>
-    <row r="77" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="15">
         <v>20</v>
       </c>
@@ -3756,7 +3790,7 @@
       </c>
       <c r="K77" s="28"/>
     </row>
-    <row r="78" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="15">
         <v>20</v>
       </c>
@@ -3789,7 +3823,7 @@
       </c>
       <c r="K78" s="28"/>
     </row>
-    <row r="79" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="15">
         <v>24</v>
       </c>
@@ -3822,7 +3856,7 @@
       </c>
       <c r="K79" s="28"/>
     </row>
-    <row r="80" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="15">
         <v>24</v>
       </c>
@@ -3855,7 +3889,7 @@
       </c>
       <c r="K80" s="28"/>
     </row>
-    <row r="81" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="15">
         <v>24</v>
       </c>
@@ -3888,7 +3922,7 @@
       </c>
       <c r="K81" s="28"/>
     </row>
-    <row r="82" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="15">
         <v>24</v>
       </c>
@@ -3923,7 +3957,7 @@
         <v>1793</v>
       </c>
     </row>
-    <row r="83" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="15">
         <v>24</v>
       </c>
@@ -3956,7 +3990,7 @@
       </c>
       <c r="K83" s="28"/>
     </row>
-    <row r="84" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="15">
         <v>24</v>
       </c>
@@ -3991,7 +4025,7 @@
         <v>1820</v>
       </c>
     </row>
-    <row r="85" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="15">
         <v>24</v>
       </c>
@@ -4024,7 +4058,7 @@
       </c>
       <c r="K85" s="28"/>
     </row>
-    <row r="86" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="15">
         <v>24</v>
       </c>
@@ -4057,7 +4091,7 @@
       </c>
       <c r="K86" s="28"/>
     </row>
-    <row r="87" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="15">
         <v>24</v>
       </c>
@@ -4090,7 +4124,7 @@
       </c>
       <c r="K87" s="28"/>
     </row>
-    <row r="88" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="15">
         <v>28</v>
       </c>
@@ -4123,7 +4157,7 @@
       </c>
       <c r="K88" s="28"/>
     </row>
-    <row r="89" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="15">
         <v>28</v>
       </c>
@@ -4156,7 +4190,7 @@
       </c>
       <c r="K89" s="28"/>
     </row>
-    <row r="90" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="15">
         <v>28</v>
       </c>
@@ -4189,7 +4223,7 @@
       </c>
       <c r="K90" s="28"/>
     </row>
-    <row r="91" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="15">
         <v>28</v>
       </c>
@@ -4224,7 +4258,7 @@
         <v>2120</v>
       </c>
     </row>
-    <row r="92" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="15">
         <v>28</v>
       </c>
@@ -4257,7 +4291,7 @@
       </c>
       <c r="K92" s="28"/>
     </row>
-    <row r="93" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="15">
         <v>28</v>
       </c>
@@ -4292,7 +4326,7 @@
         <v>2330</v>
       </c>
     </row>
-    <row r="94" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="15">
         <v>28</v>
       </c>
@@ -4325,7 +4359,7 @@
       </c>
       <c r="K94" s="28"/>
     </row>
-    <row r="95" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="15">
         <v>28</v>
       </c>
@@ -4358,7 +4392,7 @@
       </c>
       <c r="K95" s="28"/>
     </row>
-    <row r="96" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="15">
         <v>28</v>
       </c>
@@ -4391,7 +4425,7 @@
       </c>
       <c r="K96" s="28"/>
     </row>
-    <row r="97" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="15">
         <v>28</v>
       </c>
@@ -4424,7 +4458,7 @@
       </c>
       <c r="K97" s="28"/>
     </row>
-    <row r="98" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="15">
         <v>30</v>
       </c>
@@ -4457,7 +4491,7 @@
       </c>
       <c r="K98" s="28"/>
     </row>
-    <row r="99" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="15">
         <v>30</v>
       </c>
@@ -4490,7 +4524,7 @@
       </c>
       <c r="K99" s="28"/>
     </row>
-    <row r="100" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="15">
         <v>30</v>
       </c>
@@ -4523,7 +4557,7 @@
       </c>
       <c r="K100" s="28"/>
     </row>
-    <row r="101" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="15">
         <v>30</v>
       </c>
@@ -4558,7 +4592,7 @@
         <v>2215</v>
       </c>
     </row>
-    <row r="102" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="15">
         <v>30</v>
       </c>
@@ -4591,7 +4625,7 @@
       </c>
       <c r="K102" s="28"/>
     </row>
-    <row r="103" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="15">
         <v>30</v>
       </c>
@@ -4626,7 +4660,7 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="104" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="15">
         <v>30</v>
       </c>
@@ -4661,7 +4695,7 @@
         <v>2490</v>
       </c>
     </row>
-    <row r="105" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="15">
         <v>30</v>
       </c>
@@ -4694,7 +4728,7 @@
       </c>
       <c r="K105" s="28"/>
     </row>
-    <row r="106" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="15">
         <v>30</v>
       </c>
@@ -4727,7 +4761,7 @@
       </c>
       <c r="K106" s="28"/>
     </row>
-    <row r="107" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="15">
         <v>30</v>
       </c>
@@ -4760,7 +4794,7 @@
       </c>
       <c r="K107" s="28"/>
     </row>
-    <row r="108" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="15">
         <v>32</v>
       </c>
@@ -4793,7 +4827,7 @@
       </c>
       <c r="K108" s="28"/>
     </row>
-    <row r="109" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A109" s="15">
         <v>32</v>
       </c>
@@ -4826,7 +4860,7 @@
       </c>
       <c r="K109" s="28"/>
     </row>
-    <row r="110" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="15">
         <v>32</v>
       </c>
@@ -4859,7 +4893,7 @@
       </c>
       <c r="K110" s="28"/>
     </row>
-    <row r="111" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="15">
         <v>32</v>
       </c>
@@ -4894,7 +4928,7 @@
         <v>2420</v>
       </c>
     </row>
-    <row r="112" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="15">
         <v>32</v>
       </c>
@@ -4927,7 +4961,7 @@
       </c>
       <c r="K112" s="28"/>
     </row>
-    <row r="113" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" s="15">
         <v>32</v>
       </c>
@@ -4960,7 +4994,7 @@
       </c>
       <c r="K113" s="28"/>
     </row>
-    <row r="114" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" s="15">
         <v>32</v>
       </c>
@@ -4995,7 +5029,7 @@
         <v>2950</v>
       </c>
     </row>
-    <row r="115" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="15">
         <v>32</v>
       </c>
@@ -5028,7 +5062,7 @@
       </c>
       <c r="K115" s="28"/>
     </row>
-    <row r="116" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="15">
         <v>32</v>
       </c>
@@ -5061,7 +5095,7 @@
       </c>
       <c r="K116" s="28"/>
     </row>
-    <row r="117" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A117" s="15">
         <v>32</v>
       </c>
@@ -5094,7 +5128,7 @@
       </c>
       <c r="K117" s="28"/>
     </row>
-    <row r="118" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A118" s="15">
         <v>36</v>
       </c>
@@ -5127,7 +5161,7 @@
       </c>
       <c r="K118" s="28"/>
     </row>
-    <row r="119" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" s="15">
         <v>36</v>
       </c>
@@ -5160,7 +5194,7 @@
       </c>
       <c r="K119" s="28"/>
     </row>
-    <row r="120" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A120" s="15">
         <v>36</v>
       </c>
@@ -5193,7 +5227,7 @@
       </c>
       <c r="K120" s="28"/>
     </row>
-    <row r="121" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A121" s="15">
         <v>36</v>
       </c>
@@ -5226,7 +5260,7 @@
       </c>
       <c r="K121" s="28"/>
     </row>
-    <row r="122" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A122" s="15">
         <v>36</v>
       </c>
@@ -5259,7 +5293,7 @@
       </c>
       <c r="K122" s="28"/>
     </row>
-    <row r="123" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A123" s="15">
         <v>36</v>
       </c>
@@ -5294,7 +5328,7 @@
         <v>3270</v>
       </c>
     </row>
-    <row r="124" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="15">
         <v>36</v>
       </c>
@@ -5327,7 +5361,7 @@
       </c>
       <c r="K124" s="28"/>
     </row>
-    <row r="125" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A125" s="15">
         <v>36</v>
       </c>
@@ -5360,7 +5394,7 @@
       </c>
       <c r="K125" s="28"/>
     </row>
-    <row r="126" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A126" s="15">
         <v>36</v>
       </c>
@@ -5393,7 +5427,7 @@
       </c>
       <c r="K126" s="28"/>
     </row>
-    <row r="127" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A127" s="15">
         <v>40</v>
       </c>
@@ -5426,7 +5460,7 @@
       </c>
       <c r="K127" s="28"/>
     </row>
-    <row r="128" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A128" s="15">
         <v>40</v>
       </c>
@@ -5459,7 +5493,7 @@
       </c>
       <c r="K128" s="28"/>
     </row>
-    <row r="129" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A129" s="15">
         <v>40</v>
       </c>
@@ -5492,7 +5526,7 @@
       </c>
       <c r="K129" s="28"/>
     </row>
-    <row r="130" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A130" s="15">
         <v>40</v>
       </c>
@@ -5525,7 +5559,7 @@
       </c>
       <c r="K130" s="28"/>
     </row>
-    <row r="131" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A131" s="15">
         <v>40</v>
       </c>
@@ -5558,7 +5592,7 @@
       </c>
       <c r="K131" s="28"/>
     </row>
-    <row r="132" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A132" s="15">
         <v>40</v>
       </c>
@@ -5591,7 +5625,7 @@
       </c>
       <c r="K132" s="28"/>
     </row>
-    <row r="133" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A133" s="15">
         <v>40</v>
       </c>
@@ -5624,7 +5658,7 @@
       </c>
       <c r="K133" s="28"/>
     </row>
-    <row r="134" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A134" s="15">
         <v>40</v>
       </c>
@@ -5657,7 +5691,7 @@
       </c>
       <c r="K134" s="28"/>
     </row>
-    <row r="135" spans="1:11" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A135" s="15">
         <v>40</v>
       </c>
@@ -5690,7 +5724,7 @@
       </c>
       <c r="K135" s="28"/>
     </row>
-    <row r="136" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="15"/>
       <c r="B136" s="13"/>
       <c r="C136" s="21"/>
@@ -5717,15 +5751,18 @@
   <dimension ref="A1:C87"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="7" max="7" width="17.140625" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="27" t="s">
         <v>5</v>
       </c>
@@ -5736,79 +5773,74 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="23" t="s">
-        <v>16</v>
+    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="31">
+        <v>1636.8</v>
       </c>
       <c r="B2" s="23">
         <v>2000</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="23" t="s">
-        <v>16</v>
+    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="31">
+        <v>1473.2</v>
       </c>
       <c r="B3" s="23">
         <v>1800</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="23" t="s">
-        <v>16</v>
+    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="31">
+        <v>1309.4000000000001</v>
       </c>
       <c r="B4" s="23">
         <v>1600</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="23" t="s">
-        <v>16</v>
-      </c>
+    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="31"/>
       <c r="B5" s="23">
         <v>1500</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="23" t="s">
-        <v>16</v>
+    <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="31">
+        <v>1145.8</v>
       </c>
       <c r="B6" s="23">
         <v>1400</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="23" t="s">
-        <v>16</v>
+    <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="31">
+        <v>982</v>
       </c>
       <c r="B7" s="23">
         <v>1200</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="23" t="s">
-        <v>16</v>
-      </c>
+    <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="23">
         <v>1100</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="23" t="s">
-        <v>16</v>
+    <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="31">
+        <v>818.4</v>
       </c>
       <c r="B9" s="23">
         <v>1000</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="23" t="s">
-        <v>16</v>
+    <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="31">
+        <v>736.6</v>
       </c>
       <c r="B10" s="23">
         <v>900</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="23">
         <v>654.79999999999995</v>
       </c>
@@ -5819,7 +5851,7 @@
         <v>3684.0205710068726</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
         <v>16</v>
       </c>
@@ -5828,7 +5860,7 @@
       </c>
       <c r="C12" s="29"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="23">
         <v>581</v>
       </c>
@@ -5839,7 +5871,7 @@
         <v>2650</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="23" t="s">
         <v>16</v>
       </c>
@@ -5848,7 +5880,7 @@
       </c>
       <c r="C14" s="29"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="23" t="s">
         <v>16</v>
       </c>
@@ -5857,7 +5889,7 @@
       </c>
       <c r="C15" s="29"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="23">
         <v>515.6</v>
       </c>
@@ -5868,7 +5900,7 @@
         <v>2280</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="23" t="s">
         <v>16</v>
       </c>
@@ -5877,7 +5909,7 @@
       </c>
       <c r="C17" s="29"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="23">
         <v>458.4</v>
       </c>
@@ -5888,7 +5920,7 @@
         <v>1880</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="23" t="s">
         <v>16</v>
       </c>
@@ -5897,7 +5929,7 @@
       </c>
       <c r="C19" s="29"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="23">
         <v>409.2</v>
       </c>
@@ -5908,7 +5940,7 @@
         <v>1512</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="23">
         <v>368.2</v>
       </c>
@@ -5919,7 +5951,7 @@
         <v>1270</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="23">
         <v>327.39999999999998</v>
       </c>
@@ -5930,7 +5962,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="23">
         <v>290.60000000000002</v>
       </c>
@@ -5941,7 +5973,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="23" t="s">
         <v>16</v>
       </c>
@@ -5950,7 +5982,7 @@
       </c>
       <c r="C24" s="29"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="23">
         <v>257.8</v>
       </c>
@@ -5961,7 +5993,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="23" t="s">
         <v>16</v>
       </c>
@@ -5970,7 +6002,7 @@
       </c>
       <c r="C26" s="29"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="23">
         <v>229.2</v>
       </c>
@@ -5981,7 +6013,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="23">
         <v>204.6</v>
       </c>
@@ -5992,7 +6024,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="23">
         <v>184</v>
       </c>
@@ -6003,7 +6035,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="23">
         <v>163.6</v>
       </c>
@@ -6014,7 +6046,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="23">
         <v>147.19999999999999</v>
       </c>
@@ -6025,7 +6057,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="23">
         <v>130.80000000000001</v>
       </c>
@@ -6036,7 +6068,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="23">
         <v>114.6</v>
       </c>
@@ -6047,7 +6079,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="23">
         <v>102.2</v>
       </c>
@@ -6058,7 +6090,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="23">
         <v>90</v>
       </c>
@@ -6069,7 +6101,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="23">
         <v>73.599999999999994</v>
       </c>
@@ -6078,7 +6110,7 @@
       </c>
       <c r="C36" s="29"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="23">
         <v>61.8</v>
       </c>
@@ -6087,7 +6119,7 @@
       </c>
       <c r="C37" s="29"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="23">
         <v>51.4</v>
       </c>
@@ -6096,7 +6128,7 @@
       </c>
       <c r="C38" s="29"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="23">
         <v>40.799999999999997</v>
       </c>
@@ -6105,7 +6137,7 @@
       </c>
       <c r="C39" s="29"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="23">
         <v>32.6</v>
       </c>
@@ -6114,7 +6146,7 @@
       </c>
       <c r="C40" s="29"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="23">
         <v>26</v>
       </c>
@@ -6123,7 +6155,7 @@
       </c>
       <c r="C41" s="29"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="25">
         <v>20.399999999999999</v>
       </c>
@@ -6132,7 +6164,7 @@
       </c>
       <c r="C42" s="29"/>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="25">
         <v>15.4</v>
       </c>
@@ -6141,7 +6173,7 @@
       </c>
       <c r="C43" s="29"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="26" t="s">
         <v>16</v>
       </c>
@@ -6150,158 +6182,159 @@
       </c>
       <c r="C44" s="29"/>
     </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B59">
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B60">
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B61">
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B62">
         <v>3.7</v>
       </c>
     </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B63">
         <v>4.5999999999999996</v>
       </c>
     </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B64">
         <v>5.8</v>
       </c>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B65">
         <v>6.6</v>
       </c>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B66">
         <v>8.1999999999999993</v>
       </c>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B67">
         <v>10</v>
       </c>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B68">
         <v>11.4</v>
       </c>
     </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B69">
         <v>12.7</v>
       </c>
     </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B70">
         <v>14.6</v>
       </c>
     </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B71">
         <v>16.399999999999999</v>
       </c>
     </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B72">
         <v>18.2</v>
       </c>
     </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B73">
         <v>20.5</v>
       </c>
     </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B74">
         <v>22.7</v>
       </c>
     </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B75">
         <v>25.4</v>
       </c>
     </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B76">
         <v>28.6</v>
       </c>
     </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B77">
         <v>32.200000000000003</v>
       </c>
     </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B78">
         <v>36.299999999999997</v>
       </c>
     </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B79">
         <v>40.9</v>
       </c>
     </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B80">
         <v>45.4</v>
       </c>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B81">
         <v>50.8</v>
       </c>
     </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B82">
         <v>57.2</v>
       </c>
     </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B83">
         <v>64.5</v>
       </c>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B84">
         <v>72.599999999999994</v>
       </c>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6309,16 +6342,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G35" sqref="G1:N35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="8.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.140625" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
         <v>5</v>
       </c>
@@ -6329,49 +6365,47 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="23" t="s">
-        <v>16</v>
+    <row r="2" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A2" s="32">
+        <v>1763</v>
       </c>
       <c r="B2" s="23">
         <v>2000</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="23" t="s">
-        <v>16</v>
+    <row r="3" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="32">
+        <v>1586.8</v>
       </c>
       <c r="B3" s="23">
         <v>1800</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="23" t="s">
-        <v>16</v>
+    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="31">
+        <v>1410.4</v>
       </c>
       <c r="B4" s="23">
         <v>1600</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="23" t="s">
-        <v>16</v>
-      </c>
+    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="33"/>
       <c r="B5" s="23">
         <v>1500</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="23" t="s">
-        <v>16</v>
+    <row r="6" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A6" s="32">
+        <v>1234.2</v>
       </c>
       <c r="B6" s="23">
         <v>1400</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="23">
-        <v>1064.2</v>
+    <row r="7" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A7" s="32">
+        <v>1057.8</v>
       </c>
       <c r="B7" s="23">
         <v>1200</v>
@@ -6380,7 +6414,7 @@
         <v>5210.2438413096279</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
         <v>16</v>
       </c>
@@ -6389,7 +6423,7 @@
       </c>
       <c r="C8" s="30"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="23">
         <v>881.4</v>
       </c>
@@ -6401,19 +6435,19 @@
       </c>
       <c r="D9" s="30"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="23">
         <v>793.4</v>
       </c>
       <c r="B10" s="23">
         <v>900</v>
       </c>
-      <c r="C10" s="31">
+      <c r="C10" s="29">
         <v>3110</v>
       </c>
       <c r="D10" s="30"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="23">
         <v>705.2</v>
       </c>
@@ -6426,7 +6460,7 @@
       <c r="D11" s="30"/>
       <c r="E11" s="30"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
         <v>16</v>
       </c>
@@ -6434,7 +6468,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="23">
         <v>625.79999999999995</v>
       </c>
@@ -6445,7 +6479,7 @@
         <v>2190</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="23" t="s">
         <v>16</v>
       </c>
@@ -6453,7 +6487,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="23" t="s">
         <v>16</v>
       </c>
@@ -6461,7 +6495,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="23">
         <v>555.20000000000005</v>
       </c>
@@ -6472,7 +6506,7 @@
         <v>1760</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="23" t="s">
         <v>16</v>
       </c>
@@ -6480,7 +6514,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="23">
         <v>493.6</v>
       </c>
@@ -6491,7 +6525,7 @@
         <v>1440</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="23" t="s">
         <v>16</v>
       </c>
@@ -6499,7 +6533,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="23">
         <v>440.6</v>
       </c>
@@ -6510,7 +6544,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="23">
         <v>396.6</v>
       </c>
@@ -6521,7 +6555,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="23">
         <v>352.6</v>
       </c>
@@ -6532,7 +6566,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="23">
         <v>312.8</v>
       </c>
@@ -6543,7 +6577,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="23" t="s">
         <v>16</v>
       </c>
@@ -6551,7 +6585,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="23">
         <v>277.60000000000002</v>
       </c>
@@ -6562,7 +6596,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="23" t="s">
         <v>16</v>
       </c>
@@ -6570,7 +6604,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="23">
         <v>246.8</v>
       </c>
@@ -6581,7 +6615,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="23">
         <v>220.4</v>
       </c>
@@ -6592,7 +6626,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="23">
         <v>198.2</v>
       </c>
@@ -6603,7 +6637,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="23">
         <v>176.2</v>
       </c>
@@ -6614,7 +6648,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="23">
         <v>158.6</v>
       </c>
@@ -6625,7 +6659,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="23">
         <v>141</v>
       </c>
@@ -6636,7 +6670,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="23">
         <v>123.4</v>
       </c>
@@ -6647,7 +6681,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="23">
         <v>110.2</v>
       </c>
@@ -6659,7 +6693,7 @@
         <v>177.5</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="23">
         <v>96.8</v>
       </c>
@@ -6670,7 +6704,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="23">
         <v>79.2</v>
       </c>
@@ -6678,7 +6712,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="23">
         <v>66</v>
       </c>
@@ -6686,7 +6720,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="23">
         <v>55.4</v>
       </c>
@@ -6694,7 +6728,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="23">
         <v>44</v>
       </c>
@@ -6702,7 +6736,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="23">
         <v>35.200000000000003</v>
       </c>
@@ -6710,7 +6744,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="23">
         <v>28</v>
       </c>
@@ -6718,7 +6752,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="23" t="s">
         <v>16</v>
       </c>
@@ -6726,7 +6760,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="23" t="s">
         <v>16</v>
       </c>
@@ -6734,7 +6768,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="24" t="s">
         <v>16</v>
       </c>
@@ -6752,15 +6786,18 @@
   <dimension ref="A1:C87"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="H1" sqref="H1:J33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="8" max="8" width="17.140625" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="27" t="s">
         <v>5</v>
       </c>
@@ -6771,31 +6808,31 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="23" t="s">
-        <v>16</v>
+    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="31">
+        <v>1706</v>
       </c>
       <c r="B2" s="23">
         <v>2000</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="23" t="s">
-        <v>16</v>
+    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="31">
+        <v>1535.4</v>
       </c>
       <c r="B3" s="23">
         <v>1800</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="23" t="s">
-        <v>16</v>
+    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="31">
+        <v>1364.8</v>
       </c>
       <c r="B4" s="23">
         <v>1600</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="23" t="s">
         <v>16</v>
       </c>
@@ -6803,23 +6840,23 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="23" t="s">
-        <v>16</v>
+    <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="31">
+        <v>1194.2</v>
       </c>
       <c r="B6" s="23">
         <v>1400</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="23" t="s">
-        <v>16</v>
+    <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="31">
+        <v>1023.6</v>
       </c>
       <c r="B7" s="23">
         <v>1200</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="23" t="s">
         <v>16</v>
       </c>
@@ -6827,15 +6864,15 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="23" t="s">
-        <v>16</v>
+    <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="31">
+        <v>853</v>
       </c>
       <c r="B9" s="23">
         <v>1000</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="23">
         <v>767.6</v>
       </c>
@@ -6846,7 +6883,7 @@
         <v>3669.7999999999997</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="23">
         <v>682.4</v>
       </c>
@@ -6857,7 +6894,7 @@
         <v>3422</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
         <v>16</v>
       </c>
@@ -6866,7 +6903,7 @@
       </c>
       <c r="C12" s="29"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="23">
         <v>605.6</v>
       </c>
@@ -6877,7 +6914,7 @@
         <v>2580</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="23" t="s">
         <v>16</v>
       </c>
@@ -6886,7 +6923,7 @@
       </c>
       <c r="C14" s="29"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="23" t="s">
         <v>16</v>
       </c>
@@ -6895,7 +6932,7 @@
       </c>
       <c r="C15" s="29"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="23">
         <v>537.4</v>
       </c>
@@ -6906,7 +6943,7 @@
         <v>2080</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="23" t="s">
         <v>16</v>
       </c>
@@ -6915,7 +6952,7 @@
       </c>
       <c r="C17" s="29"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="23">
         <v>477.6</v>
       </c>
@@ -6926,7 +6963,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="23" t="s">
         <v>16</v>
       </c>
@@ -6935,7 +6972,7 @@
       </c>
       <c r="C19" s="29"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="23">
         <v>426.4</v>
       </c>
@@ -6946,7 +6983,7 @@
         <v>1420</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="23">
         <v>383.8</v>
       </c>
@@ -6957,7 +6994,7 @@
         <v>1190</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="23">
         <v>341.2</v>
       </c>
@@ -6968,7 +7005,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="23">
         <v>302.8</v>
       </c>
@@ -6979,7 +7016,7 @@
         <v>790</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="23" t="s">
         <v>16</v>
       </c>
@@ -6988,7 +7025,7 @@
       </c>
       <c r="C24" s="29"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="23">
         <v>268.60000000000002</v>
       </c>
@@ -6999,7 +7036,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="23" t="s">
         <v>16</v>
       </c>
@@ -7008,7 +7045,7 @@
       </c>
       <c r="C26" s="29"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="23">
         <v>238.8</v>
       </c>
@@ -7019,7 +7056,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="23">
         <v>213.2</v>
       </c>
@@ -7030,7 +7067,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="23">
         <v>191.8</v>
       </c>
@@ -7041,7 +7078,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="23">
         <v>170.6</v>
       </c>
@@ -7052,7 +7089,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="23">
         <v>153.4</v>
       </c>
@@ -7063,7 +7100,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="23">
         <v>136.4</v>
       </c>
@@ -7074,7 +7111,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="23">
         <v>119.4</v>
       </c>
@@ -7085,7 +7122,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="23">
         <v>106.6</v>
       </c>
@@ -7096,7 +7133,7 @@
         <v>192.5</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="23">
         <v>93.8</v>
       </c>
@@ -7107,7 +7144,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="23">
         <v>76.599999999999994</v>
       </c>
@@ -7116,7 +7153,7 @@
       </c>
       <c r="C36" s="29"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="23">
         <v>63.8</v>
       </c>
@@ -7125,7 +7162,7 @@
       </c>
       <c r="C37" s="29"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="23">
         <v>53.6</v>
       </c>
@@ -7134,7 +7171,7 @@
       </c>
       <c r="C38" s="29"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="23">
         <v>42.6</v>
       </c>
@@ -7142,7 +7179,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="23">
         <v>34</v>
       </c>
@@ -7150,7 +7187,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="23">
         <v>27.2</v>
       </c>
@@ -7158,7 +7195,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="25">
         <v>21</v>
       </c>
@@ -7166,7 +7203,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="25" t="s">
         <v>16</v>
       </c>
@@ -7174,7 +7211,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="26" t="s">
         <v>16</v>
       </c>
@@ -7182,152 +7219,152 @@
         <v>16</v>
       </c>
     </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B59">
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B60">
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B61">
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B62">
         <v>3.7</v>
       </c>
     </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B63">
         <v>4.5999999999999996</v>
       </c>
     </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B64">
         <v>5.8</v>
       </c>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B65">
         <v>6.6</v>
       </c>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B66">
         <v>8.1999999999999993</v>
       </c>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B67">
         <v>10</v>
       </c>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B68">
         <v>11.4</v>
       </c>
     </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B69">
         <v>12.7</v>
       </c>
     </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B70">
         <v>14.6</v>
       </c>
     </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B71">
         <v>16.399999999999999</v>
       </c>
     </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B72">
         <v>18.2</v>
       </c>
     </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B73">
         <v>20.5</v>
       </c>
     </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B74">
         <v>22.7</v>
       </c>
     </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B75">
         <v>25.4</v>
       </c>
     </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B76">
         <v>28.6</v>
       </c>
     </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B77">
         <v>32.200000000000003</v>
       </c>
     </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B78">
         <v>36.299999999999997</v>
       </c>
     </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B79">
         <v>40.9</v>
       </c>
     </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B80">
         <v>45.4</v>
       </c>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B81">
         <v>50.8</v>
       </c>
     </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B82">
         <v>57.2</v>
       </c>
     </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B83">
         <v>64.5</v>
       </c>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B84">
         <v>72.599999999999994</v>
       </c>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
         <v>18</v>
       </c>

</xml_diff>